<commit_message>
Updating models - new data feeds added e85, interim pricing and freight cost
</commit_message>
<xml_diff>
--- a/DataFeeds/DataSources.xlsx
+++ b/DataFeeds/DataSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4BB1AD-7515-4CB3-B56D-DC11CB0A9303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C313CD-C3D3-4D3D-B139-8D0F217342F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Source</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>OECD</t>
+  </si>
+  <si>
+    <t>E85</t>
+  </si>
+  <si>
+    <t>https://afdc.energy.gov/fuels/prices.html</t>
+  </si>
+  <si>
+    <t>E85 &gt;&gt; Download button</t>
+  </si>
+  <si>
+    <t>N to Q and AK &gt;&gt; Sum</t>
+  </si>
+  <si>
+    <t>Freight Cost</t>
+  </si>
+  <si>
+    <t>From Ben - Historical File "Reference: Monthly Netback Testing.xlsx"</t>
   </si>
 </sst>
 </file>
@@ -433,21 +451,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="64.26953125" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -475,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -489,7 +507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -503,7 +521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -514,7 +532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -528,7 +546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -542,7 +560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -551,6 +569,34 @@
       </c>
       <c r="C8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mine netback model added
</commit_message>
<xml_diff>
--- a/DataFeeds/DataSources.xlsx
+++ b/DataFeeds/DataSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C313CD-C3D3-4D3D-B139-8D0F217342F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F97E01-28C0-4C70-BF7C-E368F3D028AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>